<commit_message>
data: add 2023-03-23 notices
</commit_message>
<xml_diff>
--- a/data/position_notices/2023-03-23.xlsx
+++ b/data/position_notices/2023-03-23.xlsx
@@ -466,39 +466,39 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>股票名称</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>股票代码</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>公告标题</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>公告日期</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>公告发布时间</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>公告链接</t>
         </is>
@@ -530,17 +530,14 @@
           <t>2023-03-23 15:39:20:000</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>https://data.eastmoney.com/notices/detail/600461/AN202303231584503523.html</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 

</xml_diff>